<commit_message>
some data is slightly changed for the tutorial #393
</commit_message>
<xml_diff>
--- a/docs/tutorials/data/1D_BoundaryConditions.xlsx
+++ b/docs/tutorials/data/1D_BoundaryConditions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\d-hydro\educations\Delft3D-FM 1D2D RHU\Courses_2022\Nov22_DSD_ASIA\1D2D_fluvial_Delft3DFM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\checkouts\hydrolib-core\docs\tutorials\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE2CD5D-1EAC-40FD-90C2-F5F55DD05674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE8734E-D068-4861-8756-6D29FF50C41C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DCB2408D-5191-44A1-A72C-3F9B7E270894}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,8 +40,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -74,9 +73,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,12 +394,12 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -408,128 +408,143 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>40909</v>
+      <c r="A2" s="2">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>40909.25</v>
+      <c r="A3" s="2">
+        <f>6*60</f>
+        <v>360</v>
       </c>
       <c r="B3">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>40909.5</v>
+      <c r="A4" s="2">
+        <f>6*60+A3</f>
+        <v>720</v>
       </c>
       <c r="B4">
         <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>40909.75</v>
+      <c r="A5" s="2">
+        <f t="shared" ref="A5:A17" si="0">6*60+A4</f>
+        <v>1080</v>
       </c>
       <c r="B5">
         <v>800</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>40910</v>
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>1440</v>
       </c>
       <c r="B6">
         <v>1600</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>40910.25</v>
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>1800</v>
       </c>
       <c r="B7">
         <v>6400</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>40910.5</v>
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>2160</v>
       </c>
       <c r="B8">
         <v>12800</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>40910.75</v>
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>2520</v>
       </c>
       <c r="B9">
         <v>15000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>40911</v>
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>2880</v>
       </c>
       <c r="B10">
         <v>12800</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>40911.25</v>
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>3240</v>
       </c>
       <c r="B11">
         <v>6400</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>40911.5</v>
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>3600</v>
       </c>
       <c r="B12">
         <v>1600</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>40911.75</v>
+      <c r="A13" s="2">
+        <f t="shared" si="0"/>
+        <v>3960</v>
       </c>
       <c r="B13">
         <v>800</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>40912</v>
+      <c r="A14" s="2">
+        <f t="shared" si="0"/>
+        <v>4320</v>
       </c>
       <c r="B14">
         <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>40912.25</v>
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>4680</v>
       </c>
       <c r="B15">
         <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>40912.5</v>
+      <c r="A16" s="2">
+        <f t="shared" si="0"/>
+        <v>5040</v>
       </c>
       <c r="B16">
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>40918</v>
+      <c r="A17" s="2">
+        <f>132*60+A16</f>
+        <v>12960</v>
       </c>
       <c r="B17">
         <v>100</v>

</xml_diff>